<commit_message>
Sourcing Controllers and Initial Dash work
</commit_message>
<xml_diff>
--- a/Total Mercy Versioning Plan.xlsx
+++ b/Total Mercy Versioning Plan.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="MVP - v1.0" sheetId="2" r:id="rId1"/>
-    <sheet name="v2.0+" sheetId="3" r:id="rId2"/>
+    <sheet name="Current" sheetId="4" r:id="rId1"/>
+    <sheet name="MVP - v1.0" sheetId="2" r:id="rId2"/>
+    <sheet name="v2.0+" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="117">
   <si>
     <r>
       <t>·</t>
@@ -2455,6 +2456,27 @@
         <rFont val="Times New Roman"/>
       </rPr>
       <t>STRETCH - Mercy Stats/Map</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>§</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>STRECTCH - Have current view link change color</t>
     </r>
   </si>
 </sst>
@@ -2529,8 +2551,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2599,7 +2629,7 @@
       <alignment horizontal="left" vertical="center" indent="6"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2617,6 +2647,10 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2634,6 +2668,10 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2963,10 +3001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A61"/>
+  <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:A13"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3035,243 +3073,233 @@
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A13" s="7"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="7"/>
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
+      <c r="A15" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="2" t="s">
-        <v>18</v>
+      <c r="A16" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="3" t="s">
-        <v>19</v>
+      <c r="A17" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="3" t="s">
-        <v>20</v>
+      <c r="A18" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="4" t="s">
-        <v>21</v>
+      <c r="A19" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="2" t="s">
-        <v>109</v>
+      <c r="A20" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="3" t="s">
-        <v>22</v>
+      <c r="A21" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="2" t="s">
-        <v>25</v>
+      <c r="A23" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="3" t="s">
-        <v>26</v>
+      <c r="A24" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="3" t="s">
-        <v>27</v>
+      <c r="A25" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="4" t="s">
-        <v>28</v>
+      <c r="A26" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="5" t="s">
-        <v>29</v>
+      <c r="A27" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="5" t="s">
-        <v>32</v>
+      <c r="A30" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="6" t="s">
-        <v>33</v>
+      <c r="A31" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="4" t="s">
-        <v>34</v>
+      <c r="A32" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="5" t="s">
-        <v>35</v>
+      <c r="A33" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="2" t="s">
-        <v>48</v>
+      <c r="A34" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="3" t="s">
-        <v>26</v>
+      <c r="A35" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="3" t="s">
-        <v>27</v>
+      <c r="A36" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="4" t="s">
-        <v>55</v>
+      <c r="A39" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="6" t="s">
-        <v>22</v>
+      <c r="A41" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="5" t="s">
-        <v>57</v>
+      <c r="A42" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="2" t="s">
-        <v>64</v>
+      <c r="A43" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="3" t="s">
-        <v>26</v>
+      <c r="A44" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="3" t="s">
-        <v>27</v>
+      <c r="A45" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="4" t="s">
-        <v>65</v>
+      <c r="A46" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="5" t="s">
-        <v>66</v>
+      <c r="A47" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="6" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="6" t="s">
-        <v>52</v>
+      <c r="A50" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="6" t="s">
-        <v>69</v>
+      <c r="A51" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="4" t="s">
-        <v>70</v>
+      <c r="A52" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="5" t="s">
-        <v>71</v>
+      <c r="A53" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="2" t="s">
-        <v>75</v>
+      <c r="A54" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="3" t="s">
-        <v>76</v>
+      <c r="A55" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="A57" s="10"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="3" t="s">
-        <v>81</v>
+      <c r="A58" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="10"/>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="2" t="s">
+      <c r="A59" s="2" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3288,10 +3316,335 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A82"/>
+  <dimension ref="A1:A61"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:XFD82"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="103.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="7"/>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="10"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A83"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3300,395 +3653,400 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="4" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="5" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="6" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="2" t="s">
+    <row r="9" spans="1:1">
+      <c r="A9" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="2" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="3" t="s">
-        <v>106</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="2" t="s">
-        <v>110</v>
+      <c r="A13" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:1">
+      <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="4" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="8" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:1">
+      <c r="A23" s="6" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="9" t="s">
+    <row r="26" spans="1:1">
+      <c r="A26" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:1">
+      <c r="A27" s="5" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:1">
+      <c r="A30" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="6" t="s">
+    <row r="31" spans="1:1">
+      <c r="A31" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="8" t="s">
+    <row r="32" spans="1:1">
+      <c r="A32" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:1">
+      <c r="A33" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="3" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:1">
+      <c r="A35" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="5" t="s">
+    <row r="36" spans="1:1">
+      <c r="A36" s="5" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="4" t="s">
+    <row r="40" spans="1:1">
+      <c r="A40" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="5" t="s">
+    <row r="41" spans="1:1">
+      <c r="A41" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="4" t="s">
+    <row r="42" spans="1:1">
+      <c r="A42" s="4" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:1">
+      <c r="A46" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="3" t="s">
+    <row r="47" spans="1:1">
+      <c r="A47" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="4" t="s">
+    <row r="48" spans="1:1">
+      <c r="A48" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="5" t="s">
+    <row r="49" spans="1:1">
+      <c r="A49" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="6" t="s">
+    <row r="50" spans="1:1">
+      <c r="A50" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:1">
+      <c r="A51" s="2" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="4" t="s">
+    <row r="55" spans="1:1">
+      <c r="A55" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:1">
+      <c r="A56" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="3" t="s">
+    <row r="57" spans="1:1">
+      <c r="A57" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:1">
+      <c r="A58" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="3" t="s">
+    <row r="59" spans="1:1">
+      <c r="A59" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:1">
+      <c r="A61" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:1">
+      <c r="A62" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="3" t="s">
+    <row r="63" spans="1:1">
+      <c r="A63" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:1">
+      <c r="A64" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="3" t="s">
+    <row r="65" spans="1:1">
+      <c r="A65" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:1">
+      <c r="A66" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="3" t="s">
+    <row r="67" spans="1:1">
+      <c r="A67" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="4" t="s">
+    <row r="68" spans="1:1">
+      <c r="A68" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:1">
+      <c r="A69" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:1">
+      <c r="A71" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:1">
+      <c r="A72" s="2" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:1">
+      <c r="A75" s="2" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="7"/>
-    </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="7"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="2" t="s">
+    <row r="80" spans="1:1">
+      <c r="A80" s="2" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="2" t="s">
+    <row r="83" spans="1:1">
+      <c r="A83" s="2" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>